<commit_message>
Fannie Mae fuzz data
</commit_message>
<xml_diff>
--- a/PLDI-2012/raw_data/fuzz2/input_data.xlsx
+++ b/PLDI-2012/raw_data/fuzz2/input_data.xlsx
@@ -1,18 +1,52 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370"/>
+    <workbookView xWindow="9440" yWindow="6180" windowWidth="27800" windowHeight="14380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>col</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -349,284 +383,313 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="8" width="19" customWidth="1"/>
-    <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.5" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="11" max="11" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
         <v>12</v>
       </c>
-      <c r="B1">
+      <c r="C1">
         <v>13</v>
       </c>
-      <c r="C1">
+      <c r="D1">
         <v>14</v>
       </c>
-      <c r="D1">
+      <c r="E1">
         <v>15</v>
       </c>
-      <c r="E1">
+      <c r="F1">
         <v>16</v>
       </c>
-      <c r="F1">
+      <c r="G1">
         <v>18</v>
       </c>
-      <c r="G1">
+      <c r="H1">
         <v>19</v>
       </c>
-      <c r="H1">
+      <c r="I1">
         <v>21</v>
       </c>
-      <c r="I1">
+      <c r="J1">
         <v>22</v>
       </c>
-      <c r="J1">
+      <c r="K1">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>1427602155.6800001</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>340926355.50999999</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>985666.54999992996</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>30000000</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>-51786608.799999997</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>1515501799.8699999</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>-392700000</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>1124090364.1500001</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>-33376095</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>1003368420.86137</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
         <v>1398800851.3299999</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>338965688.91000003</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>-45752811.060000002</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>30000000</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>-50601311.960000001</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>1447283759.3800001</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>-383100000</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>1096925174.6300001</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>-32201025</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>1009991810.1331199</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
         <v>1361974149.3</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>332114255.61000001</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>537985.220000003</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>30000000</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>-60473972.810000002</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>1447134855.77</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>-384700000</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>1062434855.77</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>-20015625</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>1018613403.99804</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
         <v>1305498328.77</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>325268233.58999997</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>44875817.619999997</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>35000000</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>-53616441.740000002</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>1451068426.29</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>-412700000</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>1038368426.29</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>-20015625</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>1026703455.38108</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
         <v>1240524717.05</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>319819483.18000001</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>34063116.799999997</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>40000000</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>-60834434.380000003</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>1370267325.97</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>-379300000</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>990967325.97000003</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>-20015625</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>1029174575.11606</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
         <v>4188377156.31001</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>1012006300.03</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>-44319159.290000103</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>90000000</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>-162861893.56999999</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>4409920415.02001</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>-1160500000</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>3283450394.5500102</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>-85592745</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>1010658958.98808</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
         <v>3588029419.4499998</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>956934340.63999999</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>146268235.09</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>85000000</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>-193292161.31999999</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>3988593763.0700002</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>-1105900000</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>2873504780.98</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>-57815625</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>1031977291.48773</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -636,9 +699,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -648,8 +716,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>